<commit_message>
Bumped Version to 1.1, updated xlsx example and README
</commit_message>
<xml_diff>
--- a/examples/emi_import.xlsx
+++ b/examples/emi_import.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20225"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="28028"/>
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="280" yWindow="520" windowWidth="28220" windowHeight="11960"/>
+    <workbookView xWindow="280" yWindow="520" windowWidth="32820" windowHeight="12240"/>
   </bookViews>
   <sheets>
     <sheet name="datas" sheetId="1" r:id="rId1"/>
@@ -19,44 +19,39 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
-  <si>
-    <t>Libellé Segment</t>
-  </si>
-  <si>
-    <t>CP-Ville</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Description</t>
   </si>
   <si>
-    <t>31490 - BRAX</t>
-  </si>
-  <si>
-    <t>3340 - BESSAY SUR ALLIER</t>
-  </si>
-  <si>
-    <t>FOOBAR - SEMI MARATHON DE ST WITZ</t>
-  </si>
-  <si>
-    <t>FESTIVAL ROCK’ELA  DE L'ASSOCIATION LA FOULEE BRAXEENNE</t>
-  </si>
-  <si>
-    <t>2 E TOURNOI JEUNES U 13 DU CLUB SPORTIF DE BESSAY</t>
-  </si>
-  <si>
-    <t>Chupa chups gummi bears cupcake brownie jelly dessert sugar plum tootsie roll. Chupa chups gummi bears cotton candy brownie donut gingerbread wafer sweet tiramisu. Gingerbread chocolate bar halvah soufflé candy lemon drops sesame snaps dessert muffin. Cake ice cream lemon drops gummies oat cake cotton candy dragée. Macaroon powder cupcake marzipan chocolate bar. Tart applicake dragée bonbon biscuit. Cake liquorice soufflé wafer carrot cake pie chupa chups unerdwear.com jelly beans. Jujubes cupcake chocolate apple pie applicake macaroon chupa chups. Pie marzipan brownie jelly beans. Dragée tiramisu unerdwear.com tiramisu toffee bear claw cupcake. Biscuit cheesecake ice cream macaroon jujubes jelly jelly-o. Cake bonbon wafer biscuit sugar plum soufflé carrot cake.
-Brownie cotton candy halvah topping. Oat cake bear claw gingerbread fruitcake macaroon gummi bears apple pie danish cake. Icing chocolate lollipop wafer cupcake croissant liquorice. Applicake muffin chupa chups pudding topping tart icing oat cake. Icing ice cream carrot cake cupcake pudding bonbon cotton candy apple pie. Cotton candy icing chocolate cake jelly apple pie. Cookie icing bear claw. Macaroon powder gingerbread muffin dessert cupcake. Croissant toffee tiramisu oat cake. Gummies sweet donut oat cake pastry ice cream topping cupcake. Topping topping cotton candy fruitcake wafer danish. Sweet chocolate bar oat cake pie powder chocolate bar.</t>
-  </si>
-  <si>
-    <t>Fugiat blue bottle keytar aesthetic est synth. Trust fund voluptate sunt ugh. Vegan dreamcatcher small batch mlkshk. Tote bag Banksy you probably haven't heard of them, tofu bicycle rights Truffaut wayfarers pickled sunt consectetur raw denim plaid ethical laboris nostrud. Reprehenderit biodiesel whatever mlkshk, quinoa put a bird on it meh. Four loko aliqua selvage, tattooed occaecat proident squid vegan polaroid craft beer Wes Anderson. PBR art party butcher labore Truffaut raw denim.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">On quitte l'Afrique du Sud pour les Etats-Unis, mais il s'agit toujours, pour Blomkamp, de saisir un certain état de violence sociale et politique et d'en proposer une projection fictionnelle futuriste effroyable, dans laquelle les droïdes jouent un rôle de premier plan. Soit ici un monde devenu tellement pollué et infesté de microbes que les nantis, au milieu du XXIe siècle, l'ont quitté pour migrer dans un vaisseau nommé Elysium. (copy from : http://www.lemonde.fr/culture/article/2013/08/13/elysium-sur-terre-les-damnes-dans-les-airs-l-elite_3460659_3246.html)
- </t>
+    <t>Event Name</t>
+  </si>
+  <si>
+    <t>Start Time</t>
+  </si>
+  <si>
+    <t>End Time</t>
+  </si>
+  <si>
+    <t>Event Location (if not St Johns)</t>
+  </si>
+  <si>
+    <t>Example Event</t>
+  </si>
+  <si>
+    <t>Example Event 2</t>
+  </si>
+  <si>
+    <t>Sydney Opera House</t>
+  </si>
+  <si>
+    <t>Big Ben London</t>
+  </si>
+  <si>
+    <t>See an opera</t>
+  </si>
+  <si>
+    <t>Watch the clock strike</t>
   </si>
 </sst>
 </file>
@@ -64,9 +59,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="dd/mm/yyyy\ hh:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="m/d/yy\ h:mm;@"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Tahoma"/>
@@ -75,6 +70,12 @@
       <b/>
       <sz val="10"/>
       <name val="Tahoma"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -97,17 +98,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="top"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -410,73 +412,79 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D2" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="71.6640625" customWidth="1"/>
-    <col min="2" max="2" width="28.6640625" customWidth="1"/>
-    <col min="3" max="3" width="20.6640625" customWidth="1"/>
-    <col min="4" max="4" width="226.83203125" customWidth="1"/>
+    <col min="2" max="2" width="30.5" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="17.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="75.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
     </row>
-    <row r="2" spans="1:4" ht="26">
+    <row r="2" spans="1:5" ht="15">
       <c r="A2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="4">
+        <v>42875.645833333336</v>
+      </c>
+      <c r="D2" s="4">
+        <v>42875.729166666664</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15">
+      <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="3">
-        <v>41356</v>
-      </c>
-      <c r="D2" s="4" t="s">
+      <c r="B3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="4">
+        <v>42872.5</v>
+      </c>
+      <c r="D3" s="4">
+        <v>42872.625</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="78">
-      <c r="A3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="3">
-        <v>41356</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>9</v>
-      </c>
+    <row r="4" spans="1:5">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
     </row>
-    <row r="4" spans="1:4" ht="52">
-      <c r="A4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="3">
-        <v>41384</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>11</v>
-      </c>
+    <row r="5" spans="1:5">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Primary: Added proper id generation for locations and events. Other minor edits.
</commit_message>
<xml_diff>
--- a/examples/emi_import.xlsx
+++ b/examples/emi_import.xlsx
@@ -33,9 +33,6 @@
     <t>End Time</t>
   </si>
   <si>
-    <t>Event Location (if not St Johns)</t>
-  </si>
-  <si>
     <t>Example Event</t>
   </si>
   <si>
@@ -52,6 +49,9 @@
   </si>
   <si>
     <t>Watch the clock strike</t>
+  </si>
+  <si>
+    <t>Event Location</t>
   </si>
 </sst>
 </file>
@@ -61,7 +61,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yy\ h:mm;@"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Tahoma"/>
@@ -76,6 +76,18 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Tahoma"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="11"/>
+      <name val="Tahoma"/>
     </font>
   </fonts>
   <fills count="2">
@@ -95,8 +107,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -112,7 +136,19 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="13">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -415,7 +451,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -432,7 +468,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>2</v>
@@ -446,10 +482,10 @@
     </row>
     <row r="2" spans="1:5" ht="15">
       <c r="A2" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C2" s="4">
         <v>42875.645833333336</v>
@@ -458,15 +494,15 @@
         <v>42875.729166666664</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15">
       <c r="A3" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3" s="4">
         <v>42872.5</v>
@@ -475,7 +511,7 @@
         <v>42872.625</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -488,6 +524,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>